<commit_message>
udpated data and 1 gaph caption
</commit_message>
<xml_diff>
--- a/data/production.xlsx
+++ b/data/production.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliottlegendre/Documents/prive/Footsteps/footsteps/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808243E8-D688-E04C-80B7-CBE1D6134D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E485A821-515B-CC4D-8B89-B515F8C20496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15460" xr2:uid="{CBF956DE-54A9-734E-90A0-7EF75042D42E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Yield</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>dimanche, janvier 22, 2023</t>
+  </si>
+  <si>
+    <t>dimanche, mars 26, 2023</t>
+  </si>
+  <si>
+    <t>Brad Peat</t>
+  </si>
+  <si>
+    <t>samedi, avril 01, 2023</t>
+  </si>
+  <si>
+    <t>EQUILUX II</t>
   </si>
 </sst>
 </file>
@@ -483,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC98B898-7ED1-EA43-80FD-DE7ABC346C2D}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,6 +698,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>